<commit_message>
Planning & screenshots planning
</commit_message>
<xml_diff>
--- a/Planning & Assetlist.xlsx
+++ b/Planning & Assetlist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="555">
   <si>
     <t>Code Name</t>
   </si>
@@ -1682,6 +1682,9 @@
   </si>
   <si>
     <t>Medium House #4</t>
+  </si>
+  <si>
+    <t>Testing Game</t>
   </si>
 </sst>
 </file>
@@ -2496,6 +2499,12 @@
     <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2588,12 +2597,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2908,8 +2911,8 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:B4"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -2925,10 +2928,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="98" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="121"/>
+      <c r="B1" s="123"/>
       <c r="C1" s="93" t="s">
         <v>61</v>
       </c>
@@ -2958,14 +2961,14 @@
       <c r="B2" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="137" t="s">
+      <c r="C2" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="139"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="141"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
@@ -2975,30 +2978,30 @@
       <c r="B3" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="136"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="138"/>
     </row>
     <row r="4" spans="1:9" s="18" customFormat="1">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="120" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="152" t="s">
+      <c r="B4" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="131" t="s">
+      <c r="C4" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="133"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="135"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1">
@@ -3008,14 +3011,14 @@
       <c r="B5" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="122" t="s">
+      <c r="C5" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="123"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
-      <c r="H5" s="124"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="126"/>
       <c r="I5" s="116" t="s">
         <v>62</v>
       </c>
@@ -3023,14 +3026,14 @@
     <row r="6" spans="1:9" s="11" customFormat="1">
       <c r="A6" s="111"/>
       <c r="B6" s="119"/>
-      <c r="C6" s="122" t="s">
+      <c r="C6" s="124" t="s">
         <v>533</v>
       </c>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="124"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="126"/>
       <c r="I6" s="116"/>
     </row>
     <row r="7" spans="1:9" s="104" customFormat="1">
@@ -3409,30 +3412,32 @@
       <c r="G35" s="33" t="s">
         <v>481</v>
       </c>
-      <c r="H35" s="8"/>
+      <c r="H35" s="8" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="36" spans="1:9">
       <c r="D36" s="7" t="s">
         <v>401</v>
       </c>
       <c r="E36" s="6"/>
-      <c r="F36" s="128" t="s">
+      <c r="F36" s="130" t="s">
         <v>541</v>
       </c>
-      <c r="G36" s="129"/>
-      <c r="H36" s="130"/>
+      <c r="G36" s="131"/>
+      <c r="H36" s="132"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="C37" s="125" t="s">
+      <c r="C37" s="127" t="s">
         <v>551</v>
       </c>
-      <c r="D37" s="126"/>
-      <c r="E37" s="127"/>
-      <c r="F37" s="128" t="s">
+      <c r="D37" s="128"/>
+      <c r="E37" s="129"/>
+      <c r="F37" s="130" t="s">
         <v>551</v>
       </c>
-      <c r="G37" s="129"/>
-      <c r="H37" s="130"/>
+      <c r="G37" s="131"/>
+      <c r="H37" s="132"/>
     </row>
     <row r="38" spans="1:9" s="11" customFormat="1">
       <c r="A38" s="111" t="s">
@@ -3672,8 +3677,8 @@
   <dimension ref="A1:N77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -3763,7 +3768,7 @@
       <c r="K2" s="66" t="s">
         <v>200</v>
       </c>
-      <c r="L2" s="140" t="s">
+      <c r="L2" s="142" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3781,7 +3786,7 @@
       <c r="I3" s="85"/>
       <c r="J3" s="85"/>
       <c r="K3" s="85"/>
-      <c r="L3" s="141"/>
+      <c r="L3" s="143"/>
     </row>
     <row r="4" spans="1:12" s="21" customFormat="1">
       <c r="A4" s="85"/>
@@ -3797,7 +3802,7 @@
       <c r="I4" s="85"/>
       <c r="J4" s="85"/>
       <c r="K4" s="85"/>
-      <c r="L4" s="141"/>
+      <c r="L4" s="143"/>
     </row>
     <row r="5" spans="1:12" s="21" customFormat="1">
       <c r="A5" s="85"/>
@@ -3813,7 +3818,7 @@
       <c r="I5" s="85"/>
       <c r="J5" s="85"/>
       <c r="K5" s="85"/>
-      <c r="L5" s="141"/>
+      <c r="L5" s="143"/>
     </row>
     <row r="6" spans="1:12" s="21" customFormat="1">
       <c r="A6" s="85"/>
@@ -3829,7 +3834,7 @@
       <c r="I6" s="85"/>
       <c r="J6" s="85"/>
       <c r="K6" s="85"/>
-      <c r="L6" s="141"/>
+      <c r="L6" s="143"/>
     </row>
     <row r="7" spans="1:12" s="21" customFormat="1">
       <c r="A7" s="85"/>
@@ -3845,7 +3850,7 @@
       <c r="I7" s="85"/>
       <c r="J7" s="85"/>
       <c r="K7" s="85"/>
-      <c r="L7" s="141"/>
+      <c r="L7" s="143"/>
     </row>
     <row r="8" spans="1:12" s="21" customFormat="1">
       <c r="A8" s="85"/>
@@ -3861,7 +3866,7 @@
       <c r="I8" s="85"/>
       <c r="J8" s="85"/>
       <c r="K8" s="85"/>
-      <c r="L8" s="141"/>
+      <c r="L8" s="143"/>
     </row>
     <row r="9" spans="1:12" s="21" customFormat="1">
       <c r="A9" s="85"/>
@@ -3877,7 +3882,7 @@
       <c r="I9" s="85"/>
       <c r="J9" s="85"/>
       <c r="K9" s="85"/>
-      <c r="L9" s="141"/>
+      <c r="L9" s="143"/>
     </row>
     <row r="10" spans="1:12" s="21" customFormat="1">
       <c r="A10" s="85"/>
@@ -3893,7 +3898,7 @@
       <c r="I10" s="85"/>
       <c r="J10" s="85"/>
       <c r="K10" s="85"/>
-      <c r="L10" s="141"/>
+      <c r="L10" s="143"/>
     </row>
     <row r="11" spans="1:12" s="21" customFormat="1">
       <c r="A11" s="85"/>
@@ -3909,7 +3914,7 @@
       <c r="I11" s="85"/>
       <c r="J11" s="85"/>
       <c r="K11" s="85"/>
-      <c r="L11" s="142"/>
+      <c r="L11" s="144"/>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
@@ -3940,7 +3945,7 @@
         <v>71</v>
       </c>
       <c r="K12" s="16"/>
-      <c r="L12" s="143" t="s">
+      <c r="L12" s="145" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3958,7 +3963,7 @@
       <c r="I13" s="24"/>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
-      <c r="L13" s="144"/>
+      <c r="L13" s="146"/>
     </row>
     <row r="14" spans="1:12" s="60" customFormat="1">
       <c r="A14" s="60" t="s">
@@ -3991,7 +3996,7 @@
       <c r="K14" s="66" t="s">
         <v>200</v>
       </c>
-      <c r="L14" s="145"/>
+      <c r="L14" s="147"/>
     </row>
     <row r="15" spans="1:12" s="21" customFormat="1">
       <c r="A15" s="85"/>
@@ -4007,7 +4012,7 @@
       <c r="I15" s="85"/>
       <c r="J15" s="85"/>
       <c r="K15" s="85"/>
-      <c r="L15" s="141"/>
+      <c r="L15" s="143"/>
     </row>
     <row r="16" spans="1:12" s="21" customFormat="1">
       <c r="A16" s="85"/>
@@ -4023,7 +4028,7 @@
       <c r="I16" s="85"/>
       <c r="J16" s="85"/>
       <c r="K16" s="85"/>
-      <c r="L16" s="141"/>
+      <c r="L16" s="143"/>
     </row>
     <row r="17" spans="1:12" s="21" customFormat="1">
       <c r="A17" s="85"/>
@@ -4039,7 +4044,7 @@
       <c r="I17" s="85"/>
       <c r="J17" s="85"/>
       <c r="K17" s="85"/>
-      <c r="L17" s="141"/>
+      <c r="L17" s="143"/>
     </row>
     <row r="18" spans="1:12" s="21" customFormat="1">
       <c r="A18" s="85"/>
@@ -4055,7 +4060,7 @@
       <c r="I18" s="85"/>
       <c r="J18" s="85"/>
       <c r="K18" s="85"/>
-      <c r="L18" s="142"/>
+      <c r="L18" s="144"/>
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1">
       <c r="A19" s="2" t="s">
@@ -4088,7 +4093,7 @@
       <c r="K19" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="L19" s="143"/>
+      <c r="L19" s="145"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="24"/>
@@ -4104,7 +4109,7 @@
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
-      <c r="L20" s="144"/>
+      <c r="L20" s="146"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="24"/>
@@ -4120,7 +4125,7 @@
       <c r="I21" s="24"/>
       <c r="J21" s="24"/>
       <c r="K21" s="24"/>
-      <c r="L21" s="144"/>
+      <c r="L21" s="146"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="24"/>
@@ -4136,7 +4141,7 @@
       <c r="I22" s="24"/>
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
-      <c r="L22" s="146"/>
+      <c r="L22" s="148"/>
     </row>
     <row r="23" spans="1:12" s="60" customFormat="1">
       <c r="A23" s="60" t="s">
@@ -4167,7 +4172,7 @@
         <v>74</v>
       </c>
       <c r="K23" s="66"/>
-      <c r="L23" s="145"/>
+      <c r="L23" s="147"/>
     </row>
     <row r="24" spans="1:12" s="21" customFormat="1">
       <c r="A24" s="85"/>
@@ -4183,7 +4188,7 @@
       <c r="I24" s="85"/>
       <c r="J24" s="85"/>
       <c r="K24" s="85"/>
-      <c r="L24" s="141"/>
+      <c r="L24" s="143"/>
     </row>
     <row r="25" spans="1:12" s="21" customFormat="1">
       <c r="A25" s="85"/>
@@ -4199,7 +4204,7 @@
       <c r="I25" s="85"/>
       <c r="J25" s="85"/>
       <c r="K25" s="85"/>
-      <c r="L25" s="141"/>
+      <c r="L25" s="143"/>
     </row>
     <row r="26" spans="1:12" s="21" customFormat="1">
       <c r="A26" s="85"/>
@@ -4215,7 +4220,7 @@
       <c r="I26" s="85"/>
       <c r="J26" s="85"/>
       <c r="K26" s="85"/>
-      <c r="L26" s="142"/>
+      <c r="L26" s="144"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="2" t="s">
@@ -6090,7 +6095,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -7313,7 +7318,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -7332,20 +7337,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="148"/>
+      <c r="B1" s="150"/>
       <c r="C1" s="22"/>
-      <c r="D1" s="147" t="s">
+      <c r="D1" s="149" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="148"/>
+      <c r="E1" s="150"/>
       <c r="F1" s="57"/>
-      <c r="G1" s="149" t="s">
+      <c r="G1" s="151" t="s">
         <v>206</v>
       </c>
-      <c r="H1" s="150"/>
+      <c r="H1" s="152"/>
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>

</xml_diff>